<commit_message>
Feat: pycharm environment update
</commit_message>
<xml_diff>
--- a/tiktok/input.xlsx
+++ b/tiktok/input.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agayo\Desktop\크몽\dev\tiktok\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agayo\Desktop\크몽\kmong_crawler\tiktok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB1A22A-0026-4870-A2DC-05EBF45EB48A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143FEC6C-C30C-4928-BDA4-56514E6224C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{47365BA8-54E1-4CEA-A455-25E2B6F5099D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>https://www.tiktok.com/@sand.tagious/video/7151454532369665326?is_copy_url=1&amp;is_from_webapp=v1&amp;item_id=7151454532369665326</t>
+    <t>https://www.tiktok.com/@feifango/video/7142110239976869121?is_copy_url=1&amp;is_from_webapp=v1&amp;item_id=7142110239976869121</t>
   </si>
 </sst>
 </file>

</xml_diff>